<commit_message>
add data to data.xlsx
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -1,14 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22130"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ignac\Desktop\DCOPF\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6AE2C543-CBE9-498E-B6AF-2A639BAF5C3A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
+    <sheet name="gen" sheetId="1" r:id="rId1"/>
+    <sheet name="nodes" sheetId="3" r:id="rId2"/>
+    <sheet name="lines" sheetId="2" r:id="rId3"/>
   </sheets>
+  <definedNames>
+    <definedName name="LOAD">nodes!$D$1:$D$5</definedName>
+    <definedName name="PMAX">nodes!$C$2:$C$5</definedName>
+    <definedName name="PMIN">nodes!$B$2:$B$5</definedName>
+  </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -18,9 +31,56 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="14">
+  <si>
+    <t>PMIN</t>
+  </si>
+  <si>
+    <t>PMAX</t>
+  </si>
+  <si>
+    <t>NODE</t>
+  </si>
+  <si>
+    <t>CV</t>
+  </si>
+  <si>
+    <t>NODE I</t>
+  </si>
+  <si>
+    <t>NUM NODE</t>
+  </si>
+  <si>
+    <t>GEN</t>
+  </si>
+  <si>
+    <t>LOAD</t>
+  </si>
+  <si>
+    <t>P</t>
+  </si>
+  <si>
+    <t>NODE J</t>
+  </si>
+  <si>
+    <t>X</t>
+  </si>
+  <si>
+    <t>FMAX</t>
+  </si>
+  <si>
+    <t>0.4</t>
+  </si>
+  <si>
+    <t>LINES</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -28,13 +88,39 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -49,8 +135,20 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -330,12 +428,181 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:D1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8E222C23-0252-4E81-BDB0-847FC5AD5336}">
+  <dimension ref="A1:J5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K13" sqref="K13:L13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1" s="1"/>
+      <c r="B1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" s="2"/>
+      <c r="D1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="H1" s="4"/>
+      <c r="I1" s="4"/>
+      <c r="J1" s="4"/>
+    </row>
+    <row r="2" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
+        <v>1</v>
+      </c>
+      <c r="B3" s="1">
+        <v>0</v>
+      </c>
+      <c r="C3" s="1">
+        <v>100</v>
+      </c>
+      <c r="D3" s="1">
+        <v>50</v>
+      </c>
+      <c r="G3">
+        <v>1</v>
+      </c>
+      <c r="H3">
+        <v>2</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="J3">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <v>2</v>
+      </c>
+      <c r="B4" s="1">
+        <v>0</v>
+      </c>
+      <c r="C4" s="1">
+        <v>100</v>
+      </c>
+      <c r="D4" s="1">
+        <v>20</v>
+      </c>
+      <c r="G4">
+        <v>2</v>
+      </c>
+      <c r="H4">
+        <v>3</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="J4">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>3</v>
+      </c>
+      <c r="B5" s="1">
+        <v>0</v>
+      </c>
+      <c r="C5" s="1">
+        <v>100</v>
+      </c>
+      <c r="D5" s="1">
+        <v>10</v>
+      </c>
+      <c r="G5">
+        <v>3</v>
+      </c>
+      <c r="H5">
+        <v>1</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="J5">
+        <v>200</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="G1:J1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06F27EB5-7F32-4586-A8A9-A07681E860C8}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>